<commit_message>
Data Driven Testing feature added in BDD framework
</commit_message>
<xml_diff>
--- a/OutputFile/Output_Results.xlsx
+++ b/OutputFile/Output_Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="64">
   <si>
     <t>FDRateOfInterest</t>
   </si>
@@ -90,6 +90,123 @@
   </si>
   <si>
     <t>1,625</t>
+  </si>
+  <si>
+    <t>25 Apr 2029</t>
+  </si>
+  <si>
+    <t>25 Mar 2027</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>26 Apr 2029</t>
+  </si>
+  <si>
+    <t>₹1,300</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>₹487,500</t>
+  </si>
+  <si>
+    <t>24,375</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>3 Years: 0 Months : 0 Days</t>
+  </si>
+  <si>
+    <t>1095</t>
+  </si>
+  <si>
+    <t>26 Apr 2027</t>
+  </si>
+  <si>
+    <t>₹4,350</t>
+  </si>
+  <si>
+    <t>363</t>
+  </si>
+  <si>
+    <t>1000000</t>
+  </si>
+  <si>
+    <t>10 Years: 6 Months : 30 Days</t>
+  </si>
+  <si>
+    <t>3865</t>
+  </si>
+  <si>
+    <t>26 Apr 2034</t>
+  </si>
+  <si>
+    <t>₹650,000</t>
+  </si>
+  <si>
+    <t>16,250</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>3 May 2024</t>
+  </si>
+  <si>
+    <t>₹0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>₹435</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>8 Years: 6 Months : 15 Days</t>
+  </si>
+  <si>
+    <t>3120</t>
+  </si>
+  <si>
+    <t>10 Nov 2032</t>
+  </si>
+  <si>
+    <t>₹552,500</t>
+  </si>
+  <si>
+    <t>8 Years: 6 Months : 0 Days</t>
+  </si>
+  <si>
+    <t>3105</t>
+  </si>
+  <si>
+    <t>26 Oct 2032</t>
+  </si>
+  <si>
+    <t>6 Years: 0 Months : 0 Days</t>
+  </si>
+  <si>
+    <t>2191</t>
+  </si>
+  <si>
+    <t>26 Apr 2030</t>
+  </si>
+  <si>
+    <t>₹390,000</t>
   </si>
 </sst>
 </file>
@@ -433,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -642,6 +759,686 @@
         <v>24</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I20" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="I21" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="I24" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="I26" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H27" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="I27" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H29" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I29" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H30" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I30" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="I31" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored Base Page class
</commit_message>
<xml_diff>
--- a/OutputFile/Output_Results.xlsx
+++ b/OutputFile/Output_Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="67">
   <si>
     <t>FDRateOfInterest</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>₹390,000</t>
+  </si>
+  <si>
+    <t>30 Apr 2029</t>
+  </si>
+  <si>
+    <t>30 Apr 2027</t>
+  </si>
+  <si>
+    <t>30 Apr 2030</t>
   </si>
 </sst>
 </file>
@@ -550,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -1439,6 +1448,151 @@
         <v>45</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G32" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H32" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I32" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G33" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H33" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="I33" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G34" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H34" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I34" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H35" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="I35" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H36" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="I36" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>